<commit_message>
finished and fixed with qr decomp
</commit_message>
<xml_diff>
--- a/Output/AllModels_final_with_plan_12000.xlsx
+++ b/Output/AllModels_final_with_plan_12000.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="245">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -62,16 +62,16 @@
     <t xml:space="preserve">[ 0.19,  0.35]</t>
   </si>
   <si>
-    <t xml:space="preserve">37.81***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[32.93, 43.41]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">111.17***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[99.96, 123.69]</t>
+    <t xml:space="preserve">37.84***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[33.00, 43.33]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111.19***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[99.90, 123.80]</t>
   </si>
   <si>
     <t xml:space="preserve">3.67***</t>
@@ -83,7 +83,7 @@
     <t xml:space="preserve">0.34**</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.17,   0.64]</t>
+    <t xml:space="preserve">[0.17,   0.65]</t>
   </si>
   <si>
     <t xml:space="preserve">Within-Person Effects</t>
@@ -146,7 +146,7 @@
     <t xml:space="preserve">1.12</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.84,   1.54]</t>
+    <t xml:space="preserve">[0.84,   1.53]</t>
   </si>
   <si>
     <t xml:space="preserve">Daily pressure experienced</t>
@@ -155,7 +155,7 @@
     <t xml:space="preserve">0.96</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 0.70,  1.31]</t>
+    <t xml:space="preserve">[ 0.69,  1.30]</t>
   </si>
   <si>
     <t xml:space="preserve">0.91</t>
@@ -176,10 +176,10 @@
     <t xml:space="preserve">[-0.14, 0.07]</t>
   </si>
   <si>
-    <t xml:space="preserve">1.97*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.01,   4.38]</t>
+    <t xml:space="preserve">1.98*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.02,   4.58]</t>
   </si>
   <si>
     <t xml:space="preserve">Daily pressure utilized (partner's view)</t>
@@ -188,7 +188,7 @@
     <t xml:space="preserve">1.49*</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 1.04,  2.33]</t>
+    <t xml:space="preserve">[ 1.05,  2.34]</t>
   </si>
   <si>
     <t xml:space="preserve">[ 0.86,  1.03]</t>
@@ -203,16 +203,16 @@
     <t xml:space="preserve">[-0.15, 0.08]</t>
   </si>
   <si>
-    <t xml:space="preserve">1.43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.59,   4.21]</t>
+    <t xml:space="preserve">1.41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.54,   4.37]</t>
   </si>
   <si>
     <t xml:space="preserve">Daily pushing experienced</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 0.71,  1.31]</t>
+    <t xml:space="preserve">[ 0.71,  1.30]</t>
   </si>
   <si>
     <t xml:space="preserve">0.99</t>
@@ -233,10 +233,10 @@
     <t xml:space="preserve">[-0.06, 0.07]</t>
   </si>
   <si>
-    <t xml:space="preserve">1.33*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1.03,   1.76]</t>
+    <t xml:space="preserve">1.34*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1.04,   1.76]</t>
   </si>
   <si>
     <t xml:space="preserve">Daily pushing utilized (partner's view)</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">1.29*</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 1.05,  1.63]</t>
+    <t xml:space="preserve">[ 1.05,  1.62]</t>
   </si>
   <si>
     <t xml:space="preserve">[ 0.90,  1.02]</t>
@@ -263,7 +263,10 @@
     <t xml:space="preserve">[ 0.00, 0.14]</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.61,   1.36]</t>
+    <t xml:space="preserve">0.92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.61,   1.37]</t>
   </si>
   <si>
     <t xml:space="preserve">Day</t>
@@ -272,10 +275,10 @@
     <t xml:space="preserve">0.86</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 0.65,  1.15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.87,  1.11]</t>
+    <t xml:space="preserve">[ 0.64,  1.16]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.88,  1.12]</t>
   </si>
   <si>
     <t xml:space="preserve">0.97</t>
@@ -287,19 +290,19 @@
     <t xml:space="preserve">[ 0.15, 0.37]</t>
   </si>
   <si>
-    <t xml:space="preserve">1.67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.78,   3.60]</t>
+    <t xml:space="preserve">1.68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.77,   3.69]</t>
   </si>
   <si>
     <t xml:space="preserve">Own Actionplan</t>
   </si>
   <si>
-    <t xml:space="preserve">9.46***</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 7.77, 11.57]</t>
+    <t xml:space="preserve">9.45***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 7.76, 11.57]</t>
   </si>
   <si>
     <t xml:space="preserve">1.32***</t>
@@ -323,7 +326,7 @@
     <t xml:space="preserve">0.87</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.46,   1.63]</t>
+    <t xml:space="preserve">[0.46,   1.62]</t>
   </si>
   <si>
     <t xml:space="preserve">Partner Actionplan</t>
@@ -332,7 +335,7 @@
     <t xml:space="preserve">1.17</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 0.96,  1.41]</t>
+    <t xml:space="preserve">[ 0.96,  1.42]</t>
   </si>
   <si>
     <t xml:space="preserve">1.08</t>
@@ -350,7 +353,10 @@
     <t xml:space="preserve">[-0.11, 0.04]</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.49,   1.54]</t>
+    <t xml:space="preserve">0.88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.49,   1.58]</t>
   </si>
   <si>
     <t xml:space="preserve">Daily weartime</t>
@@ -368,10 +374,10 @@
     <t xml:space="preserve">Mean persuasion experienced</t>
   </si>
   <si>
-    <t xml:space="preserve">1.48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.73,  3.06]</t>
+    <t xml:space="preserve">1.49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.72,  3.06]</t>
   </si>
   <si>
     <t xml:space="preserve">[ 0.74,  1.34]</t>
@@ -386,13 +392,13 @@
     <t xml:space="preserve">0.34</t>
   </si>
   <si>
-    <t xml:space="preserve">[-0.21, 0.89]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.91</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.58,   6.66]</t>
+    <t xml:space="preserve">[-0.23, 0.90]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.51,   7.72]</t>
   </si>
   <si>
     <t xml:space="preserve">Mean persuasion utilized (partner's view)</t>
@@ -401,7 +407,7 @@
     <t xml:space="preserve">1.40</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 0.69,  2.86]</t>
+    <t xml:space="preserve">[ 0.69,  2.85]</t>
   </si>
   <si>
     <t xml:space="preserve">[ 0.71,  1.28]</t>
@@ -413,13 +419,13 @@
     <t xml:space="preserve">0.23</t>
   </si>
   <si>
-    <t xml:space="preserve">[-0.33, 0.77]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.50,   7.26]</t>
+    <t xml:space="preserve">[-0.34, 0.79]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.47,   9.47]</t>
   </si>
   <si>
     <t xml:space="preserve">Mean pressure experienced</t>
@@ -431,10 +437,10 @@
     <t xml:space="preserve">[ 0.17,  0.88]</t>
   </si>
   <si>
-    <t xml:space="preserve">1.20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.85,  1.70]</t>
+    <t xml:space="preserve">1.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.86,  1.69]</t>
   </si>
   <si>
     <t xml:space="preserve">[ 0.74,   1.32]</t>
@@ -443,13 +449,13 @@
     <t xml:space="preserve">-0.30</t>
   </si>
   <si>
-    <t xml:space="preserve">[-0.84, 0.24]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.52**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[2.54, 166.38]</t>
+    <t xml:space="preserve">[-0.85, 0.25]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.35**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[2.64, 404.79]</t>
   </si>
   <si>
     <t xml:space="preserve">Mean pressure utilized (partner's view)</t>
@@ -458,58 +464,55 @@
     <t xml:space="preserve">0.49</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 0.22,  1.13]</t>
+    <t xml:space="preserve">[ 0.21,  1.14]</t>
   </si>
   <si>
     <t xml:space="preserve">0.94</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 0.66,  1.34]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.74,   1.28]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.85, 0.23]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.24,  19.50]</t>
+    <t xml:space="preserve">[ 0.66,  1.33]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.74,   1.29]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.87, 0.23]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.11,  19.86]</t>
   </si>
   <si>
     <t xml:space="preserve">Mean pushing experienced</t>
   </si>
   <si>
-    <t xml:space="preserve">1.09</t>
-  </si>
-  <si>
     <t xml:space="preserve">[ 0.38,  3.17]</t>
   </si>
   <si>
-    <t xml:space="preserve">1.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.80,  1.92]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ 0.63,   1.42]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.58, 0.97]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.12,   6.06]</t>
+    <t xml:space="preserve">1.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.80,  1.94]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 0.64,   1.44]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.57, 0.99]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.06,   5.70]</t>
   </si>
   <si>
     <t xml:space="preserve">Mean pushing utilized (partner's view)</t>
@@ -518,13 +521,13 @@
     <t xml:space="preserve">1.96</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 0.68,  5.67]</t>
+    <t xml:space="preserve">[ 0.69,  5.73]</t>
   </si>
   <si>
     <t xml:space="preserve">1.34</t>
   </si>
   <si>
-    <t xml:space="preserve">[ 0.86,  2.09]</t>
+    <t xml:space="preserve">[ 0.85,  2.11]</t>
   </si>
   <si>
     <t xml:space="preserve">1.22</t>
@@ -533,16 +536,16 @@
     <t xml:space="preserve">[ 0.82,   1.83]</t>
   </si>
   <si>
-    <t xml:space="preserve">0.35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-0.40, 1.12]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.08*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01,   0.69]</t>
+    <t xml:space="preserve">0.36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-0.41, 1.15]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.05*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.00,   0.55]</t>
   </si>
   <si>
     <t xml:space="preserve">Mean weartime</t>
@@ -578,10 +581,10 @@
     <t xml:space="preserve">[0.47, 0.78]</t>
   </si>
   <si>
-    <t xml:space="preserve">1.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.74, 1.75]</t>
+    <t xml:space="preserve">1.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.75, 1.79]</t>
   </si>
   <si>
     <t xml:space="preserve">sd(Daily persuasion experienced)</t>
@@ -590,7 +593,7 @@
     <t xml:space="preserve">0.21</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.03, 0.40]</t>
+    <t xml:space="preserve">[0.03, 0.39]</t>
   </si>
   <si>
     <t xml:space="preserve">0.11</t>
@@ -629,7 +632,7 @@
     <t xml:space="preserve">[0.04, 0.13]</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.03, 0.09]</t>
+    <t xml:space="preserve">[0.02, 0.09]</t>
   </si>
   <si>
     <t xml:space="preserve">0.07</t>
@@ -638,7 +641,7 @@
     <t xml:space="preserve">[0.01, 0.13]</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.13, 0.98]</t>
+    <t xml:space="preserve">[0.12, 0.99]</t>
   </si>
   <si>
     <t xml:space="preserve">sd(Daily pressure experienced)</t>
@@ -650,10 +653,10 @@
     <t xml:space="preserve">[0.00, 0.23]</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.00, 0.13]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.14, 2.44]</t>
+    <t xml:space="preserve">[0.00, 0.14]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.13, 2.47]</t>
   </si>
   <si>
     <t xml:space="preserve">sd(Daily pressure utilized (partner's view))</t>
@@ -662,7 +665,7 @@
     <t xml:space="preserve">0.24</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.01, 0.95]</t>
+    <t xml:space="preserve">[0.01, 0.94]</t>
   </si>
   <si>
     <t xml:space="preserve">0.06</t>
@@ -680,16 +683,13 @@
     <t xml:space="preserve">[0.00, 0.26]</t>
   </si>
   <si>
-    <t xml:space="preserve">0.81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.04, 2.70]</t>
+    <t xml:space="preserve">[0.05, 2.83]</t>
   </si>
   <si>
     <t xml:space="preserve">sd(Daily pushing experienced)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.58</t>
+    <t xml:space="preserve">0.59</t>
   </si>
   <si>
     <t xml:space="preserve">[0.31, 1.01]</t>
@@ -704,13 +704,10 @@
     <t xml:space="preserve">[0.01, 0.15]</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.00, 0.14]</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.25</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.02, 0.62]</t>
+    <t xml:space="preserve">[0.02, 0.61]</t>
   </si>
   <si>
     <t xml:space="preserve">sd(Daily pushing utilized (partner's view))</t>
@@ -722,16 +719,13 @@
     <t xml:space="preserve">[0.01, 0.50]</t>
   </si>
   <si>
-    <t xml:space="preserve">[0.00, 0.09]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.00, 0.16]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.01, 0.96]</t>
+    <t xml:space="preserve">[0.01, 0.16]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.01, 0.99]</t>
   </si>
   <si>
     <t xml:space="preserve">Additional Parameters</t>
@@ -1478,130 +1472,130 @@
         <v>82</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>52</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1610,252 +1604,252 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="8" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>50</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>60</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>67</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1865,7 +1859,7 @@
         <v>79</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1874,209 +1868,209 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="K25" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="J27" s="1" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>222</v>
+        <v>86</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>223</v>
@@ -2099,117 +2093,117 @@
         <v>228</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>229</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I29" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="D30" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>229</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>243</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>245</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>46</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>

</xml_diff>